<commit_message>
Scripts for submission version
</commit_message>
<xml_diff>
--- a/Simon classification from other papers.xlsx
+++ b/Simon classification from other papers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dcs0spb/Software/CEP_Retro/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AA0032D-A832-5149-83F5-396E25A6706C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D28B0F29-707A-4E4E-B8BA-9A07C05AB56D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -817,8 +817,8 @@
   </sheetPr>
   <dimension ref="A1:AX995"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>

</xml_diff>